<commit_message>
Automation files and API, Database layout
</commit_message>
<xml_diff>
--- a/01-Manual-Testing/Test-Cases/Login_Test_Cases.xlsx
+++ b/01-Manual-Testing/Test-Cases/Login_Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashlynnwii/Desktop/Ashlynn-QA-Portfolio/01-Manual-Testing/Test-Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E099968-2D0A-114D-ACB0-C58D28A56D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8C8329-743A-C641-967C-E67B4055153E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="840" windowWidth="24220" windowHeight="18020" xr2:uid="{FAED3FD0-4BDF-3545-99AB-5C230261F276}"/>
   </bookViews>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>